<commit_message>
update F.py & usage_example.py
</commit_message>
<xml_diff>
--- a/log/c620_op_log.xlsx
+++ b/log/c620_op_log.xlsx
@@ -488,11 +488,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>123456</t>
+          <t>123</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8620922565460205</v>
+        <v>0.8620919585227966</v>
       </c>
       <c r="C2" t="n">
         <v>0.4265280067920685</v>
@@ -504,22 +504,22 @@
         <v>0.8786906003952026</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8720481395721436</v>
+        <v>0.8718597888946533</v>
       </c>
       <c r="G2" t="n">
-        <v>97.02023315429688</v>
+        <v>97.02018737792969</v>
       </c>
       <c r="H2" t="n">
-        <v>12.55310249328613</v>
+        <v>14.78398036956787</v>
       </c>
       <c r="I2" t="n">
-        <v>12.04037284851074</v>
+        <v>12.06411457061768</v>
       </c>
       <c r="J2" t="n">
-        <v>178.1207275390625</v>
+        <v>178.1206817626953</v>
       </c>
       <c r="K2" t="n">
-        <v>194.7436828613281</v>
+        <v>194.7444610595703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update F.py & web.py
</commit_message>
<xml_diff>
--- a/log/c620_op_log.xlsx
+++ b/log/c620_op_log.xlsx
@@ -488,11 +488,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>test</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8620919585227966</v>
+        <v>0.8620922565460205</v>
       </c>
       <c r="C2" t="n">
         <v>0.4265280067920685</v>
@@ -504,22 +504,22 @@
         <v>0.8786906003952026</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8718597888946533</v>
+        <v>0.8720412254333496</v>
       </c>
       <c r="G2" t="n">
-        <v>97.02018737792969</v>
+        <v>97.02023315429688</v>
       </c>
       <c r="H2" t="n">
-        <v>14.78398036956787</v>
+        <v>12.5676794052124</v>
       </c>
       <c r="I2" t="n">
-        <v>12.06411457061768</v>
+        <v>12.04052448272705</v>
       </c>
       <c r="J2" t="n">
-        <v>178.1206817626953</v>
+        <v>178.1207275390625</v>
       </c>
       <c r="K2" t="n">
-        <v>194.7444610595703</v>
+        <v>194.7437133789062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add icg_model_svr and update config.py,F.py,usage_example.py,web.py
</commit_message>
<xml_diff>
--- a/log/c620_op_log.xlsx
+++ b/log/c620_op_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,6 +664,80 @@
         <v>194.6712646484375</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8646729588508606</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.4265280067920685</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8276968598365784</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8786906003952026</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8721588850021362</v>
+      </c>
+      <c r="G7" t="n">
+        <v>97.02021026611328</v>
+      </c>
+      <c r="H7" t="n">
+        <v>12.51860427856445</v>
+      </c>
+      <c r="I7" t="n">
+        <v>12.0368595123291</v>
+      </c>
+      <c r="J7" t="n">
+        <v>178.1204681396484</v>
+      </c>
+      <c r="K7" t="n">
+        <v>194.4346466064453</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8646729588508606</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.4265280067920685</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8276968598365784</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8786906003952026</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.8721616268157959</v>
+      </c>
+      <c r="G8" t="n">
+        <v>97.02021026611328</v>
+      </c>
+      <c r="H8" t="n">
+        <v>12.52402591705322</v>
+      </c>
+      <c r="I8" t="n">
+        <v>12.03680610656738</v>
+      </c>
+      <c r="J8" t="n">
+        <v>178.1204681396484</v>
+      </c>
+      <c r="K8" t="n">
+        <v>194.4124450683594</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update F.py usage_example.py 推薦功能要從980作為inital value
</commit_message>
<xml_diff>
--- a/log/c620_op_log.xlsx
+++ b/log/c620_op_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,6 +738,80 @@
         <v>194.4124450683594</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8646729588508606</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.4265280067920685</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8276968598365784</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8786906003952026</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.8721588850021362</v>
+      </c>
+      <c r="G9" t="n">
+        <v>97.02021026611328</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12.51860427856445</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12.0368595123291</v>
+      </c>
+      <c r="J9" t="n">
+        <v>178.1204681396484</v>
+      </c>
+      <c r="K9" t="n">
+        <v>194.4346466064453</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8646729588508606</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.4265280067920685</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8276968598365784</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8786906003952026</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.8721616268157959</v>
+      </c>
+      <c r="G10" t="n">
+        <v>97.02021026611328</v>
+      </c>
+      <c r="H10" t="n">
+        <v>12.52402591705322</v>
+      </c>
+      <c r="I10" t="n">
+        <v>12.03680610656738</v>
+      </c>
+      <c r="J10" t="n">
+        <v>178.1204681396484</v>
+      </c>
+      <c r="K10" t="n">
+        <v>194.4124450683594</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update F.py usage_example.py 修正流程運作邏輯
</commit_message>
<xml_diff>
--- a/log/c620_op_log.xlsx
+++ b/log/c620_op_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,6 +812,80 @@
         <v>194.4124450683594</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8646729588508606</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.4265280067920685</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.8276968598365784</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.8786906003952026</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.8721588850021362</v>
+      </c>
+      <c r="G11" t="n">
+        <v>97.02021026611328</v>
+      </c>
+      <c r="H11" t="n">
+        <v>12.51860427856445</v>
+      </c>
+      <c r="I11" t="n">
+        <v>12.0368595123291</v>
+      </c>
+      <c r="J11" t="n">
+        <v>178.1204681396484</v>
+      </c>
+      <c r="K11" t="n">
+        <v>194.4346466064453</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8646729588508606</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4265280067920685</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.8276968598365784</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8786906003952026</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.8721616268157959</v>
+      </c>
+      <c r="G12" t="n">
+        <v>97.02021026611328</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12.52402591705322</v>
+      </c>
+      <c r="I12" t="n">
+        <v>12.03680610656738</v>
+      </c>
+      <c r="J12" t="n">
+        <v>178.1204681396484</v>
+      </c>
+      <c r="K12" t="n">
+        <v>194.4124450683594</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>